<commit_message>
Modified power plant generation file
</commit_message>
<xml_diff>
--- a/resources/sources/powerplants/translation table.xlsx
+++ b/resources/sources/powerplants/translation table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcmel/Development/java-projects/emlab-generation2/resources/sources/powerplants/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{365FD338-7152-724F-BF35-3FA6CDA04122}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA023F6-57F7-034B-B277-95A79B558F1D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16220" xr2:uid="{64790AA3-27FA-8044-BDD5-A94A3F2AD3E6}"/>
   </bookViews>
@@ -514,7 +514,7 @@
   <dimension ref="B1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="142" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>